<commit_message>
Modified mean buffer metric
</commit_message>
<xml_diff>
--- a/excel/FactorialAnalysis_MeanResponseTime.xlsx
+++ b/excel/FactorialAnalysis_MeanResponseTime.xlsx
@@ -1073,7 +1073,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart123.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart127.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1677,11 +1677,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="67961634"/>
-        <c:axId val="33844260"/>
+        <c:axId val="98419304"/>
+        <c:axId val="21103724"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="67961634"/>
+        <c:axId val="98419304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1723,12 +1723,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="33844260"/>
+        <c:crossAx val="21103724"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="33844260"/>
+        <c:axId val="21103724"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1770,7 +1770,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="67961634"/>
+        <c:crossAx val="98419304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1798,7 +1798,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart124.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart128.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2386,11 +2386,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="57377667"/>
-        <c:axId val="119025"/>
+        <c:axId val="14235939"/>
+        <c:axId val="13247443"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="57377667"/>
+        <c:axId val="14235939"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2432,12 +2432,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="119025"/>
+        <c:crossAx val="13247443"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="119025"/>
+        <c:axId val="13247443"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2479,7 +2479,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="57377667"/>
+        <c:crossAx val="14235939"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2579,7 +2579,7 @@
   </sheetPr>
   <dimension ref="B1:AR225"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C13" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="S2" activeCellId="0" sqref="S2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added 2kr with different warmup e simduration
</commit_message>
<xml_diff>
--- a/excel/FactorialAnalysis_MeanResponseTime.xlsx
+++ b/excel/FactorialAnalysis_MeanResponseTime.xlsx
@@ -708,7 +708,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="72">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -925,10 +925,6 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="22" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1073,7 +1069,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart127.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart19.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1677,11 +1673,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="98419304"/>
-        <c:axId val="21103724"/>
+        <c:axId val="23813114"/>
+        <c:axId val="45855233"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="98419304"/>
+        <c:axId val="23813114"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1723,12 +1719,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="21103724"/>
+        <c:crossAx val="45855233"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="21103724"/>
+        <c:axId val="45855233"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1770,7 +1766,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="98419304"/>
+        <c:crossAx val="23813114"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1798,7 +1794,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart128.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart20.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2386,11 +2382,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="14235939"/>
-        <c:axId val="13247443"/>
+        <c:axId val="40675582"/>
+        <c:axId val="42024069"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="14235939"/>
+        <c:axId val="40675582"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2432,12 +2428,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="13247443"/>
+        <c:crossAx val="42024069"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="13247443"/>
+        <c:axId val="42024069"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2479,7 +2475,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="14235939"/>
+        <c:crossAx val="40675582"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2518,9 +2514,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
-      <xdr:colOff>212040</xdr:colOff>
+      <xdr:colOff>211320</xdr:colOff>
       <xdr:row>73</xdr:row>
-      <xdr:rowOff>117000</xdr:rowOff>
+      <xdr:rowOff>116280</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2528,8 +2524,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="13492440" y="9662040"/>
-        <a:ext cx="7560720" cy="3304080"/>
+        <a:off x="13495320" y="9662040"/>
+        <a:ext cx="7566840" cy="3303360"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2548,9 +2544,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
-      <xdr:colOff>172440</xdr:colOff>
+      <xdr:colOff>171720</xdr:colOff>
       <xdr:row>167</xdr:row>
-      <xdr:rowOff>160200</xdr:rowOff>
+      <xdr:rowOff>159480</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2558,8 +2554,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="11895120" y="24117840"/>
-        <a:ext cx="9118440" cy="5365800"/>
+        <a:off x="11896920" y="24117840"/>
+        <a:ext cx="9125640" cy="5365080"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2579,11 +2575,11 @@
   </sheetPr>
   <dimension ref="B1:AR225"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C13" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="S2" activeCellId="0" sqref="S2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="X25" activeCellId="0" sqref="X25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.71484375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="18.71"/>
@@ -6743,78 +6739,78 @@
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D49" s="54" t="s">
+      <c r="D49" s="38" t="s">
         <v>60</v>
       </c>
-      <c r="E49" s="55" t="n">
+      <c r="E49" s="54" t="n">
         <f aca="false">E46-SQRT(($Y$47^2)/4*5)*$X$50</f>
         <v>-1.41553096739502</v>
       </c>
-      <c r="F49" s="56" t="n">
+      <c r="F49" s="55" t="n">
         <f aca="false">F46-SQRT(($Y$47^2)/4*5)*$X$50</f>
         <v>0.0708792463505177</v>
       </c>
-      <c r="G49" s="56" t="n">
+      <c r="G49" s="55" t="n">
         <f aca="false">G46-SQRT(($Y$47^2)/4*5)*$X$50</f>
         <v>-0.0875715530819968</v>
       </c>
-      <c r="H49" s="56" t="n">
+      <c r="H49" s="55" t="n">
         <f aca="false">H46-SQRT(($Y$47^2)/4*5)*$X$50</f>
         <v>-0.392379536519395</v>
       </c>
-      <c r="I49" s="56" t="n">
+      <c r="I49" s="55" t="n">
         <f aca="false">I46-SQRT(($Y$47^2)/4*5)*$X$50</f>
         <v>-0.14319367839053</v>
       </c>
-      <c r="J49" s="56" t="n">
+      <c r="J49" s="55" t="n">
         <f aca="false">J46-SQRT(($Y$47^2)/4*5)*$X$50</f>
         <v>-0.0763003328681682</v>
       </c>
-      <c r="K49" s="56" t="n">
+      <c r="K49" s="55" t="n">
         <f aca="false">K46-SQRT(($Y$47^2)/4*5)*$X$50</f>
         <v>-0.00613841806030545</v>
       </c>
-      <c r="L49" s="56" t="n">
+      <c r="L49" s="55" t="n">
         <f aca="false">L46-SQRT(($Y$47^2)/4*5)*$X$50</f>
         <v>-0.0747092568034562</v>
       </c>
-      <c r="M49" s="56" t="n">
+      <c r="M49" s="55" t="n">
         <f aca="false">M46-SQRT(($Y$47^2)/4*5)*$X$50</f>
         <v>-0.000937258952320814</v>
       </c>
-      <c r="N49" s="56" t="n">
+      <c r="N49" s="55" t="n">
         <f aca="false">N46-SQRT(($Y$47^2)/4*5)*$X$50</f>
         <v>0.0694900925843916</v>
       </c>
-      <c r="O49" s="56" t="n">
+      <c r="O49" s="55" t="n">
         <f aca="false">O46-SQRT(($Y$47^2)/4*5)*$X$50</f>
         <v>0.0535895422678415</v>
       </c>
-      <c r="P49" s="56" t="n">
+      <c r="P49" s="55" t="n">
         <f aca="false">P46-SQRT(($Y$47^2)/4*5)*$X$50</f>
         <v>0.000691446223006613</v>
       </c>
-      <c r="Q49" s="56" t="n">
+      <c r="Q49" s="55" t="n">
         <f aca="false">Q46-SQRT(($Y$47^2)/4*5)*$X$50</f>
         <v>0.0596107817901657</v>
       </c>
-      <c r="R49" s="56" t="n">
+      <c r="R49" s="55" t="n">
         <f aca="false">R46-SQRT(($Y$47^2)/4*5)*$X$50</f>
         <v>0.0068227635840175</v>
       </c>
-      <c r="S49" s="56" t="n">
+      <c r="S49" s="55" t="n">
         <f aca="false">S46-SQRT(($Y$47^2)/4*5)*$X$50</f>
         <v>-0.0112137315089329</v>
       </c>
-      <c r="T49" s="57" t="n">
+      <c r="T49" s="56" t="n">
         <f aca="false">T46-SQRT(($Y$47^2)/4*5)*$X$50</f>
         <v>-0.0102145925802961</v>
       </c>
-      <c r="W49" s="58" t="s">
+      <c r="W49" s="57" t="s">
         <v>61</v>
       </c>
-      <c r="X49" s="58"/>
-      <c r="Y49" s="58"/>
+      <c r="X49" s="57"/>
+      <c r="Y49" s="57"/>
       <c r="AI49" s="0" t="s">
         <v>59</v>
       </c>
@@ -6826,64 +6822,64 @@
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D50" s="54"/>
-      <c r="E50" s="59" t="n">
+      <c r="D50" s="38"/>
+      <c r="E50" s="58" t="n">
         <f aca="false">E46+SQRT(($Y$47^2)/4*5)*$X$50</f>
         <v>-1.40768959728637</v>
       </c>
-      <c r="F50" s="60" t="n">
+      <c r="F50" s="59" t="n">
         <f aca="false">F46+SQRT(($Y$47^2)/4*5)*$X$50</f>
         <v>0.078720616459171</v>
       </c>
-      <c r="G50" s="60" t="n">
+      <c r="G50" s="59" t="n">
         <f aca="false">G46+SQRT(($Y$47^2)/4*5)*$X$50</f>
         <v>-0.0797301829733434</v>
       </c>
-      <c r="H50" s="60" t="n">
+      <c r="H50" s="59" t="n">
         <f aca="false">H46+SQRT(($Y$47^2)/4*5)*$X$50</f>
         <v>-0.384538166410742</v>
       </c>
-      <c r="I50" s="60" t="n">
+      <c r="I50" s="59" t="n">
         <f aca="false">I46+SQRT(($Y$47^2)/4*5)*$X$50</f>
         <v>-0.135352308281876</v>
       </c>
-      <c r="J50" s="60" t="n">
+      <c r="J50" s="59" t="n">
         <f aca="false">J46+SQRT(($Y$47^2)/4*5)*$X$50</f>
         <v>-0.0684589627595149</v>
       </c>
-      <c r="K50" s="60" t="n">
+      <c r="K50" s="59" t="n">
         <f aca="false">K46+SQRT(($Y$47^2)/4*5)*$X$50</f>
         <v>0.00170295204834787</v>
       </c>
-      <c r="L50" s="60" t="n">
+      <c r="L50" s="59" t="n">
         <f aca="false">L46+SQRT(($Y$47^2)/4*5)*$X$50</f>
         <v>-0.0668678866948029</v>
       </c>
-      <c r="M50" s="60" t="n">
+      <c r="M50" s="59" t="n">
         <f aca="false">M46+SQRT(($Y$47^2)/4*5)*$X$50</f>
         <v>0.00690411115633251</v>
       </c>
-      <c r="N50" s="60" t="n">
+      <c r="N50" s="59" t="n">
         <f aca="false">N46+SQRT(($Y$47^2)/4*5)*$X$50</f>
         <v>0.0773314626930449</v>
       </c>
-      <c r="O50" s="60" t="n">
+      <c r="O50" s="59" t="n">
         <f aca="false">O46+SQRT(($Y$47^2)/4*5)*$X$50</f>
         <v>0.0614309123764949</v>
       </c>
-      <c r="P50" s="60" t="n">
+      <c r="P50" s="59" t="n">
         <f aca="false">P46+SQRT(($Y$47^2)/4*5)*$X$50</f>
         <v>0.00853281633165993</v>
       </c>
-      <c r="Q50" s="60" t="n">
+      <c r="Q50" s="59" t="n">
         <f aca="false">Q46+SQRT(($Y$47^2)/4*5)*$X$50</f>
         <v>0.0674521518988191</v>
       </c>
-      <c r="R50" s="60" t="n">
+      <c r="R50" s="59" t="n">
         <f aca="false">R46+SQRT(($Y$47^2)/4*5)*$X$50</f>
         <v>0.0146641336926708</v>
       </c>
-      <c r="S50" s="60" t="n">
+      <c r="S50" s="59" t="n">
         <f aca="false">S46+SQRT(($Y$47^2)/4*5)*$X$50</f>
         <v>-0.00337236140027961</v>
       </c>
@@ -6923,17 +6919,17 @@
       <c r="AK52" s="14"/>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C53" s="61"/>
-      <c r="D53" s="62"/>
-      <c r="E53" s="63" t="s">
+      <c r="C53" s="60"/>
+      <c r="D53" s="61"/>
+      <c r="E53" s="62" t="s">
         <v>63</v>
       </c>
-      <c r="F53" s="63"/>
-      <c r="G53" s="63"/>
-      <c r="H53" s="63"/>
-      <c r="I53" s="63"/>
-      <c r="J53" s="63"/>
-      <c r="K53" s="63"/>
+      <c r="F53" s="62"/>
+      <c r="G53" s="62"/>
+      <c r="H53" s="62"/>
+      <c r="I53" s="62"/>
+      <c r="J53" s="62"/>
+      <c r="K53" s="62"/>
       <c r="AI53" s="0" t="s">
         <v>64</v>
       </c>
@@ -6945,15 +6941,15 @@
       </c>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C54" s="62"/>
-      <c r="D54" s="62"/>
-      <c r="E54" s="63"/>
-      <c r="F54" s="63"/>
-      <c r="G54" s="63"/>
-      <c r="H54" s="63"/>
-      <c r="I54" s="63"/>
-      <c r="J54" s="63"/>
-      <c r="K54" s="63"/>
+      <c r="C54" s="61"/>
+      <c r="D54" s="61"/>
+      <c r="E54" s="62"/>
+      <c r="F54" s="62"/>
+      <c r="G54" s="62"/>
+      <c r="H54" s="62"/>
+      <c r="I54" s="62"/>
+      <c r="J54" s="62"/>
+      <c r="K54" s="62"/>
       <c r="AI54" s="0" t="s">
         <v>64</v>
       </c>
@@ -6965,12 +6961,12 @@
       </c>
     </row>
     <row r="55" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C55" s="62"/>
-      <c r="D55" s="62"/>
-      <c r="E55" s="62"/>
-      <c r="F55" s="62"/>
-      <c r="G55" s="62"/>
-      <c r="H55" s="62"/>
+      <c r="C55" s="61"/>
+      <c r="D55" s="61"/>
+      <c r="E55" s="61"/>
+      <c r="F55" s="61"/>
+      <c r="G55" s="61"/>
+      <c r="H55" s="61"/>
       <c r="AI55" s="0" t="s">
         <v>64</v>
       </c>
@@ -6993,19 +6989,19 @@
       </c>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E57" s="64" t="s">
+      <c r="E57" s="63" t="s">
         <v>65</v>
       </c>
-      <c r="F57" s="65" t="s">
+      <c r="F57" s="64" t="s">
         <v>66</v>
       </c>
-      <c r="G57" s="65" t="s">
+      <c r="G57" s="64" t="s">
         <v>67</v>
       </c>
-      <c r="H57" s="65" t="s">
+      <c r="H57" s="64" t="s">
         <v>68</v>
       </c>
-      <c r="I57" s="66" t="s">
+      <c r="I57" s="65" t="s">
         <v>69</v>
       </c>
       <c r="AI57" s="0" t="s">
@@ -7019,21 +7015,21 @@
       </c>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E58" s="67" t="n">
-        <v>1</v>
-      </c>
-      <c r="F58" s="68" t="n">
+      <c r="E58" s="66" t="n">
+        <v>1</v>
+      </c>
+      <c r="F58" s="67" t="n">
         <f aca="false">(E58-0.5)/$E$137</f>
         <v>0.00625</v>
       </c>
-      <c r="G58" s="68" t="n">
+      <c r="G58" s="67" t="n">
         <f aca="false">_xlfn.NORM.S.INV(F58)</f>
         <v>-2.49770547441237</v>
       </c>
       <c r="H58" s="17" t="n">
         <v>-0.0778132709973807</v>
       </c>
-      <c r="I58" s="69" t="n">
+      <c r="I58" s="68" t="n">
         <f aca="false">AA5</f>
         <v>-0.00116757760054009</v>
       </c>
@@ -7604,18 +7600,18 @@
         <f aca="false">AB9</f>
         <v>0.00442332772050391</v>
       </c>
-      <c r="M78" s="70" t="s">
+      <c r="M78" s="69" t="s">
         <v>74</v>
       </c>
-      <c r="N78" s="70"/>
-      <c r="O78" s="70"/>
-      <c r="P78" s="70"/>
-      <c r="Q78" s="70"/>
-      <c r="R78" s="70"/>
-      <c r="S78" s="70"/>
-      <c r="T78" s="70"/>
-      <c r="U78" s="70"/>
-      <c r="V78" s="70"/>
+      <c r="N78" s="69"/>
+      <c r="O78" s="69"/>
+      <c r="P78" s="69"/>
+      <c r="Q78" s="69"/>
+      <c r="R78" s="69"/>
+      <c r="S78" s="69"/>
+      <c r="T78" s="69"/>
+      <c r="U78" s="69"/>
+      <c r="V78" s="69"/>
       <c r="AI78" s="0" t="s">
         <v>73</v>
       </c>
@@ -7646,18 +7642,18 @@
         <f aca="false">AB10</f>
         <v>0.00939676148632018</v>
       </c>
-      <c r="M79" s="71" t="s">
+      <c r="M79" s="70" t="s">
         <v>75</v>
       </c>
-      <c r="N79" s="71"/>
-      <c r="O79" s="71"/>
-      <c r="P79" s="71"/>
-      <c r="Q79" s="71"/>
-      <c r="R79" s="71"/>
-      <c r="S79" s="71"/>
-      <c r="T79" s="71"/>
-      <c r="U79" s="71"/>
-      <c r="V79" s="71"/>
+      <c r="N79" s="70"/>
+      <c r="O79" s="70"/>
+      <c r="P79" s="70"/>
+      <c r="Q79" s="70"/>
+      <c r="R79" s="70"/>
+      <c r="S79" s="70"/>
+      <c r="T79" s="70"/>
+      <c r="U79" s="70"/>
+      <c r="V79" s="70"/>
       <c r="AI79" s="0" t="s">
         <v>73</v>
       </c>
@@ -7688,16 +7684,16 @@
         <f aca="false">AB11</f>
         <v>0.00402754060883126</v>
       </c>
-      <c r="M80" s="71"/>
-      <c r="N80" s="71"/>
-      <c r="O80" s="71"/>
-      <c r="P80" s="71"/>
-      <c r="Q80" s="71"/>
-      <c r="R80" s="71"/>
-      <c r="S80" s="71"/>
-      <c r="T80" s="71"/>
-      <c r="U80" s="71"/>
-      <c r="V80" s="71"/>
+      <c r="M80" s="70"/>
+      <c r="N80" s="70"/>
+      <c r="O80" s="70"/>
+      <c r="P80" s="70"/>
+      <c r="Q80" s="70"/>
+      <c r="R80" s="70"/>
+      <c r="S80" s="70"/>
+      <c r="T80" s="70"/>
+      <c r="U80" s="70"/>
+      <c r="V80" s="70"/>
       <c r="AI80" s="0" t="s">
         <v>73</v>
       </c>
@@ -7728,18 +7724,18 @@
         <f aca="false">AB12</f>
         <v>0.000459678826931098</v>
       </c>
-      <c r="M81" s="72" t="s">
+      <c r="M81" s="71" t="s">
         <v>76</v>
       </c>
-      <c r="N81" s="72"/>
-      <c r="O81" s="72"/>
-      <c r="P81" s="72"/>
-      <c r="Q81" s="72"/>
-      <c r="R81" s="72"/>
-      <c r="S81" s="72"/>
-      <c r="T81" s="72"/>
-      <c r="U81" s="72"/>
-      <c r="V81" s="72"/>
+      <c r="N81" s="71"/>
+      <c r="O81" s="71"/>
+      <c r="P81" s="71"/>
+      <c r="Q81" s="71"/>
+      <c r="R81" s="71"/>
+      <c r="S81" s="71"/>
+      <c r="T81" s="71"/>
+      <c r="U81" s="71"/>
+      <c r="V81" s="71"/>
       <c r="AI81" s="0" t="s">
         <v>73</v>
       </c>
@@ -7770,16 +7766,16 @@
         <f aca="false">AB13</f>
         <v>0.0611415035604904</v>
       </c>
-      <c r="M82" s="72"/>
-      <c r="N82" s="72"/>
-      <c r="O82" s="72"/>
-      <c r="P82" s="72"/>
-      <c r="Q82" s="72"/>
-      <c r="R82" s="72"/>
-      <c r="S82" s="72"/>
-      <c r="T82" s="72"/>
-      <c r="U82" s="72"/>
-      <c r="V82" s="72"/>
+      <c r="M82" s="71"/>
+      <c r="N82" s="71"/>
+      <c r="O82" s="71"/>
+      <c r="P82" s="71"/>
+      <c r="Q82" s="71"/>
+      <c r="R82" s="71"/>
+      <c r="S82" s="71"/>
+      <c r="T82" s="71"/>
+      <c r="U82" s="71"/>
+      <c r="V82" s="71"/>
     </row>
     <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E83" s="16" t="n">
@@ -8811,7 +8807,7 @@
         <f aca="false">_xlfn.NORM.S.INV(F125)</f>
         <v>1.00999016924958</v>
       </c>
-      <c r="H125" s="68" t="n">
+      <c r="H125" s="67" t="n">
         <v>0.00939676148632018</v>
       </c>
       <c r="I125" s="19" t="n">
@@ -9072,45 +9068,45 @@
       </c>
     </row>
     <row r="141" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E141" s="63" t="s">
+      <c r="E141" s="62" t="s">
         <v>80</v>
       </c>
-      <c r="F141" s="63"/>
-      <c r="G141" s="63"/>
-      <c r="H141" s="63"/>
-      <c r="I141" s="63"/>
-      <c r="J141" s="63"/>
-      <c r="K141" s="63"/>
+      <c r="F141" s="62"/>
+      <c r="G141" s="62"/>
+      <c r="H141" s="62"/>
+      <c r="I141" s="62"/>
+      <c r="J141" s="62"/>
+      <c r="K141" s="62"/>
     </row>
     <row r="142" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E142" s="63"/>
-      <c r="F142" s="63"/>
-      <c r="G142" s="63"/>
-      <c r="H142" s="63"/>
-      <c r="I142" s="63"/>
-      <c r="J142" s="63"/>
-      <c r="K142" s="63"/>
+      <c r="E142" s="62"/>
+      <c r="F142" s="62"/>
+      <c r="G142" s="62"/>
+      <c r="H142" s="62"/>
+      <c r="I142" s="62"/>
+      <c r="J142" s="62"/>
+      <c r="K142" s="62"/>
     </row>
     <row r="145" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E145" s="64" t="s">
+      <c r="E145" s="63" t="s">
         <v>65</v>
       </c>
-      <c r="F145" s="65" t="s">
+      <c r="F145" s="64" t="s">
         <v>81</v>
       </c>
-      <c r="G145" s="66" t="s">
+      <c r="G145" s="65" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E146" s="67" t="n">
-        <v>1</v>
-      </c>
-      <c r="F146" s="68" t="n">
+      <c r="E146" s="66" t="n">
+        <v>1</v>
+      </c>
+      <c r="F146" s="67" t="n">
         <f aca="false">U$5</f>
         <v>-0.965564507854728</v>
       </c>
-      <c r="G146" s="69" t="n">
+      <c r="G146" s="68" t="n">
         <f aca="false">AA$5</f>
         <v>-0.00116757760054009</v>
       </c>

</xml_diff>